<commit_message>
added big data results
</commit_message>
<xml_diff>
--- a/itmd-521/Week-11/images/Graphs.xlsx
+++ b/itmd-521/Week-11/images/Graphs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B392AC92-3D58-43D7-AA61-5C46E6AE86AB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB73AE8-3B0D-42AC-BFAD-3974542CE7A9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SmallDataset" sheetId="1" r:id="rId1"/>
@@ -148,8 +148,17 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>combiner and without combiner</a:t>
+              <a:t>combiner and without combiner over </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" i="1" u="sng"/>
+              <a:t>SMALL DATA (one year)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -656,8 +665,17 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>combiner and without combiner</a:t>
+              <a:t>combiner and without combiner over </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" i="1" u="sng"/>
+              <a:t>BIG</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" i="1" u="sng" baseline="0"/>
+              <a:t> DATA (decade)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" i="1" u="sng"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -820,6 +838,62 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>SmallDataset_Combiner!$A$1:$F$1</c:f>
@@ -853,22 +927,22 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1707</c:v>
+                  <c:v>776</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1134</c:v>
+                  <c:v>341</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1382</c:v>
+                  <c:v>857</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>548</c:v>
+                  <c:v>387</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1386</c:v>
+                  <c:v>880</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>700</c:v>
+                  <c:v>282</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2480,8 +2554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2582,8 +2656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFF073F-5284-4616-A731-A70D561BA367}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2615,22 +2689,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>1707</v>
+        <v>776</v>
       </c>
       <c r="B2" s="1">
-        <v>1134</v>
+        <v>341</v>
       </c>
       <c r="C2" s="1">
-        <v>1382</v>
+        <v>857</v>
       </c>
       <c r="D2" s="1">
-        <v>548</v>
+        <v>387</v>
       </c>
       <c r="E2" s="1">
-        <v>1386</v>
+        <v>880</v>
       </c>
       <c r="F2" s="1">
-        <v>700</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>